<commit_message>
Added download cancellation and error display
</commit_message>
<xml_diff>
--- a/doc/todo.xlsx
+++ b/doc/todo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Priority</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Add ability to see Blob URL and other data</t>
+  </si>
+  <si>
+    <t>Add application icon</t>
+  </si>
+  <si>
+    <t>Delete downloaded file after download canceled</t>
   </si>
 </sst>
 </file>
@@ -416,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -571,6 +577,16 @@
     <row r="22" spans="2:2">
       <c r="B22" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ability to change download folder
</commit_message>
<xml_diff>
--- a/doc/todo.xlsx
+++ b/doc/todo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Priority</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Bug: cancelled download changes to "starting" when new download is started</t>
+  </si>
+  <si>
+    <t>Change folder list background to azure</t>
+  </si>
+  <si>
+    <t>Fast multi-threaded download</t>
   </si>
 </sst>
 </file>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D32"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -467,42 +473,42 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>10000</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>10000</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>10000</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>10000</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -510,7 +516,7 @@
         <v>10000</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -518,7 +524,7 @@
         <v>10000</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -526,7 +532,7 @@
         <v>10000</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -534,7 +540,7 @@
         <v>10000</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -542,7 +548,7 @@
         <v>10000</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -550,107 +556,132 @@
         <v>10000</v>
       </c>
       <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>10000</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>10000</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>10000</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>10000</v>
+      </c>
+      <c r="B16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="B13" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>10000</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="B14" t="s">
+    <row r="19" spans="1:2">
+      <c r="B19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="B15" t="s">
+    <row r="20" spans="1:2">
+      <c r="B20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
+    <row r="21" spans="1:2">
+      <c r="B21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
+    <row r="22" spans="1:2">
+      <c r="B22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
+    <row r="23" spans="1:2">
+      <c r="B23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
+    <row r="24" spans="1:2">
+      <c r="B24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="s">
+    <row r="25" spans="1:2">
+      <c r="B25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
-      <c r="B22" t="s">
+    <row r="26" spans="1:2">
+      <c r="B26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="s">
+    <row r="27" spans="1:2">
+      <c r="B27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:2">
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" t="s">
+    <row r="28" spans="1:2">
+      <c r="B28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="2:2">
-      <c r="B27" t="s">
+    <row r="29" spans="1:2">
+      <c r="B29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="2:2">
-      <c r="B28" t="s">
+    <row r="30" spans="1:2">
+      <c r="B30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:2">
-      <c r="B29" t="s">
+    <row r="31" spans="1:2">
+      <c r="B31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:2">
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" t="s">
+    <row r="32" spans="1:2">
+      <c r="B32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="2:2">
-      <c r="B32" t="s">
-        <v>32</v>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug: download state of already complete or cancelled downloads changes when new download starts
</commit_message>
<xml_diff>
--- a/doc/todo.xlsx
+++ b/doc/todo.xlsx
@@ -455,7 +455,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -473,7 +473,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>30</v>
+        <v>10000</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>

</xml_diff>